<commit_message>
JADE_Scrum.xlsx Updated sprint backlog
</commit_message>
<xml_diff>
--- a/P12/JADE_Scrum.xlsx
+++ b/P12/JADE_Scrum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/waseem/Documents/SchoolCode/cse1325/P10/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WASEE\Google Drive\College\2021\2021 Fall\cse1325\P12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AC2982-21AE-4642-B9AD-E28A76A0A772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722A0052-3D22-448D-8BF9-A98B48A6195B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="314">
   <si>
     <t>Product Name:</t>
   </si>
@@ -559,9 +559,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>--&gt; Add tasks to complete each feature for this sprint</t>
-  </si>
-  <si>
     <t>NOTE: A stand-alone assignment on threading is Nov 16-30</t>
   </si>
   <si>
@@ -971,6 +968,21 @@
   </si>
   <si>
     <t>JLabel in create order dialog</t>
+  </si>
+  <si>
+    <t>Create Edit menubar menu</t>
+  </si>
+  <si>
+    <t>Add Product button to Edit menu</t>
+  </si>
+  <si>
+    <t>Add Product button to toolbar</t>
+  </si>
+  <si>
+    <t>Implement ActionListener for Product button</t>
+  </si>
+  <si>
+    <t>In Work</t>
   </si>
 </sst>
 </file>
@@ -3234,7 +3246,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -3311,28 +3323,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3382,7 +3394,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -3456,7 +3468,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -4500,23 +4512,23 @@
   </sheetPr>
   <dimension ref="A1:AMJ62"/>
   <sheetViews>
-    <sheetView zoomScale="116" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView topLeftCell="A29" zoomScale="116" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="45.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="39.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="55.83203125" style="1" customWidth="1"/>
-    <col min="11" max="1024" width="11.5" style="1"/>
+    <col min="3" max="3" width="8.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="45.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="39.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="55.85546875" style="1" customWidth="1"/>
+    <col min="11" max="1024" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="18">
@@ -4536,12 +4548,12 @@
       </c>
       <c r="I1"/>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="16">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -4584,14 +4596,14 @@
         <v>7</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
       <c r="G5" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H5" s="5">
         <v>1001841927</v>
@@ -4904,7 +4916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
@@ -4921,7 +4933,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>32</v>
@@ -4934,7 +4946,7 @@
       </c>
       <c r="J24" s="15"/>
     </row>
-    <row r="25" spans="1:10" ht="14">
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -4951,7 +4963,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>32</v>
@@ -4964,7 +4976,7 @@
       </c>
       <c r="J25" s="15"/>
     </row>
-    <row r="26" spans="1:10" ht="14">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -4981,7 +4993,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>32</v>
@@ -4994,7 +5006,7 @@
       </c>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="1:10" ht="28">
+    <row r="27" spans="1:10" ht="38.25">
       <c r="A27" s="16" t="s">
         <v>41</v>
       </c>
@@ -5011,7 +5023,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>32</v>
@@ -5026,7 +5038,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="28">
+    <row r="28" spans="1:10" ht="25.5">
       <c r="A28" s="16" t="s">
         <v>45</v>
       </c>
@@ -5043,7 +5055,7 @@
         <v>2</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>32</v>
@@ -5058,7 +5070,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="20" customFormat="1" ht="28">
+    <row r="29" spans="1:10" s="20" customFormat="1" ht="25.5">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -5075,7 +5087,7 @@
         <v>3</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>32</v>
@@ -5090,7 +5102,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="20" customFormat="1" ht="28">
+    <row r="30" spans="1:10" s="20" customFormat="1" ht="25.5">
       <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
@@ -5107,7 +5119,7 @@
         <v>3</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>32</v>
@@ -5122,7 +5134,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="20" customFormat="1" ht="28">
+    <row r="31" spans="1:10" s="20" customFormat="1" ht="25.5">
       <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
@@ -5139,7 +5151,7 @@
         <v>3</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>32</v>
@@ -5154,7 +5166,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="14">
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
         <v>57</v>
       </c>
@@ -5171,7 +5183,7 @@
         <v>3</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>58</v>
@@ -5186,7 +5198,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:1024" ht="14">
+    <row r="33" spans="1:1024">
       <c r="A33" s="1" t="s">
         <v>62</v>
       </c>
@@ -5203,7 +5215,7 @@
         <v>3</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>58</v>
@@ -5235,7 +5247,7 @@
         <v>4</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G34" s="18" t="s">
         <v>32</v>
@@ -6264,7 +6276,7 @@
       <c r="AMI34"/>
       <c r="AMJ34"/>
     </row>
-    <row r="35" spans="1:1024" s="20" customFormat="1" ht="14">
+    <row r="35" spans="1:1024" s="20" customFormat="1">
       <c r="A35" s="16" t="s">
         <v>68</v>
       </c>
@@ -6281,7 +6293,7 @@
         <v>4</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G35" s="18" t="s">
         <v>69</v>
@@ -6294,7 +6306,7 @@
       </c>
       <c r="J35" s="19"/>
     </row>
-    <row r="36" spans="1:1024" s="20" customFormat="1" ht="14">
+    <row r="36" spans="1:1024" s="20" customFormat="1">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
@@ -6311,7 +6323,7 @@
         <v>5</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G36" s="12" t="s">
         <v>69</v>
@@ -6324,7 +6336,7 @@
       </c>
       <c r="J36" s="15"/>
     </row>
-    <row r="37" spans="1:1024" s="20" customFormat="1" ht="14">
+    <row r="37" spans="1:1024" s="20" customFormat="1">
       <c r="A37" s="1" t="s">
         <v>75</v>
       </c>
@@ -6341,7 +6353,7 @@
         <v>5</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G37" s="12" t="s">
         <v>69</v>
@@ -6356,7 +6368,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:1024" s="20" customFormat="1" ht="14">
+    <row r="38" spans="1:1024" s="20" customFormat="1">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
@@ -6373,7 +6385,7 @@
         <v>5</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G38" s="12" t="s">
         <v>80</v>
@@ -6388,7 +6400,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:1024" s="20" customFormat="1" ht="28">
+    <row r="39" spans="1:1024" s="20" customFormat="1" ht="25.5">
       <c r="A39" s="1" t="s">
         <v>84</v>
       </c>
@@ -6405,7 +6417,7 @@
         <v>5</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>80</v>
@@ -6420,7 +6432,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:1024" s="20" customFormat="1" ht="28">
+    <row r="40" spans="1:1024" s="20" customFormat="1" ht="25.5">
       <c r="A40" s="1" t="s">
         <v>88</v>
       </c>
@@ -6437,7 +6449,7 @@
         <v>5</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>80</v>
@@ -6452,7 +6464,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:1024" s="20" customFormat="1" ht="28">
+    <row r="41" spans="1:1024" s="20" customFormat="1" ht="25.5">
       <c r="A41" s="1" t="s">
         <v>92</v>
       </c>
@@ -6469,7 +6481,7 @@
         <v>5</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>80</v>
@@ -6484,7 +6496,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:1024" s="22" customFormat="1" ht="28">
+    <row r="42" spans="1:1024" s="22" customFormat="1" ht="25.5">
       <c r="A42" s="16" t="s">
         <v>95</v>
       </c>
@@ -6512,7 +6524,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:1024" ht="28">
+    <row r="43" spans="1:1024" ht="25.5">
       <c r="A43" s="16" t="s">
         <v>99</v>
       </c>
@@ -6540,7 +6552,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:1024" ht="14">
+    <row r="44" spans="1:1024" ht="25.5">
       <c r="A44" s="16" t="s">
         <v>102</v>
       </c>
@@ -6605,7 +6617,7 @@
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
     </row>
-    <row r="48" spans="1:1024" ht="28">
+    <row r="48" spans="1:1024" ht="25.5">
       <c r="A48" s="1" t="s">
         <v>108</v>
       </c>
@@ -6633,7 +6645,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="20" customFormat="1" ht="14">
+    <row r="49" spans="1:10" s="20" customFormat="1">
       <c r="A49" s="1" t="s">
         <v>112</v>
       </c>
@@ -6659,7 +6671,7 @@
       </c>
       <c r="J49" s="15"/>
     </row>
-    <row r="50" spans="1:10" ht="14">
+    <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
         <v>115</v>
       </c>
@@ -6685,7 +6697,7 @@
       </c>
       <c r="J50" s="15"/>
     </row>
-    <row r="51" spans="1:10" ht="28">
+    <row r="51" spans="1:10" ht="38.25">
       <c r="A51" s="1" t="s">
         <v>118</v>
       </c>
@@ -6711,7 +6723,7 @@
       </c>
       <c r="J51" s="15"/>
     </row>
-    <row r="52" spans="1:10" ht="14">
+    <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
         <v>121</v>
       </c>
@@ -6737,7 +6749,7 @@
       </c>
       <c r="J52" s="15"/>
     </row>
-    <row r="53" spans="1:10" ht="28">
+    <row r="53" spans="1:10" ht="25.5">
       <c r="A53" s="1" t="s">
         <v>124</v>
       </c>
@@ -6763,7 +6775,7 @@
       </c>
       <c r="J53" s="15"/>
     </row>
-    <row r="54" spans="1:10" ht="14">
+    <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
         <v>127</v>
       </c>
@@ -6817,7 +6829,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="20" customFormat="1" ht="28">
+    <row r="56" spans="1:10" s="20" customFormat="1" ht="25.5">
       <c r="A56" s="1" t="s">
         <v>134</v>
       </c>
@@ -6845,7 +6857,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="28">
+    <row r="57" spans="1:10" ht="25.5">
       <c r="A57" s="1" t="s">
         <v>138</v>
       </c>
@@ -6871,7 +6883,7 @@
       </c>
       <c r="J57" s="15"/>
     </row>
-    <row r="58" spans="1:10" ht="28">
+    <row r="58" spans="1:10" ht="25.5">
       <c r="A58" s="1" t="s">
         <v>141</v>
       </c>
@@ -6897,7 +6909,7 @@
       </c>
       <c r="J58" s="15"/>
     </row>
-    <row r="59" spans="1:10" ht="28">
+    <row r="59" spans="1:10" ht="25.5">
       <c r="A59" s="1" t="s">
         <v>144</v>
       </c>
@@ -6923,7 +6935,7 @@
       </c>
       <c r="J59" s="15"/>
     </row>
-    <row r="60" spans="1:10" ht="28">
+    <row r="60" spans="1:10" ht="38.25">
       <c r="A60" s="1" t="s">
         <v>147</v>
       </c>
@@ -6949,7 +6961,7 @@
       </c>
       <c r="J60" s="15"/>
     </row>
-    <row r="61" spans="1:10" ht="14">
+    <row r="61" spans="1:10">
       <c r="A61" s="1" t="s">
         <v>150</v>
       </c>
@@ -6975,7 +6987,7 @@
       </c>
       <c r="J61" s="15"/>
     </row>
-    <row r="62" spans="1:10" ht="28">
+    <row r="62" spans="1:10" ht="25.5">
       <c r="A62" s="1" t="s">
         <v>152</v>
       </c>
@@ -7069,13 +7081,13 @@
       <selection activeCell="B17" sqref="B17:E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="51.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="51.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="25" customFormat="1" ht="18">
@@ -7342,13 +7354,13 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="E17" s="33" t="s">
         <v>182</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -7359,13 +7371,13 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -7376,13 +7388,13 @@
         <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -7393,13 +7405,13 @@
         <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -7410,13 +7422,13 @@
         <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D21" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="E21" s="33" t="s">
         <v>187</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -7427,13 +7439,13 @@
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -7444,13 +7456,13 @@
         <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -7461,13 +7473,13 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -7478,13 +7490,13 @@
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D25" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="E25" s="33" t="s">
         <v>187</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -7495,13 +7507,13 @@
         <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -7512,13 +7524,13 @@
         <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -7529,13 +7541,13 @@
         <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -7546,13 +7558,13 @@
         <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -8184,13 +8196,13 @@
       <selection activeCell="B17" sqref="B17:F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="51.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="51.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="25" customFormat="1" ht="18">
@@ -8459,13 +8471,13 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D17" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="E17" s="33" t="s">
         <v>196</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -8476,16 +8488,16 @@
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D18" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="E18" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="F18" t="s">
         <v>199</v>
-      </c>
-      <c r="F18" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -8496,13 +8508,13 @@
         <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -8513,13 +8525,13 @@
         <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -8530,13 +8542,13 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D21" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" s="33" t="s">
         <v>203</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -8547,16 +8559,16 @@
         <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D22" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="F22" t="s">
         <v>205</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>197</v>
-      </c>
-      <c r="F22" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -8567,13 +8579,13 @@
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -8584,13 +8596,13 @@
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -8601,16 +8613,16 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D25" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="F25" t="s">
         <v>209</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="F25" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -8621,13 +8633,13 @@
         <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -8638,16 +8650,16 @@
         <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D27" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="E27" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="F27" t="s">
         <v>212</v>
-      </c>
-      <c r="E27" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="F27" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -8658,13 +8670,13 @@
         <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E28" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -9304,13 +9316,13 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="51.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="51.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="25" customFormat="1" ht="18">
@@ -9579,13 +9591,13 @@
         <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D17" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="E17" s="33" t="s">
         <v>215</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -9596,13 +9608,13 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -9613,13 +9625,13 @@
         <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -9630,13 +9642,13 @@
         <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -9647,13 +9659,13 @@
         <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -9664,13 +9676,13 @@
         <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -9681,13 +9693,13 @@
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -9698,13 +9710,13 @@
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -9715,13 +9727,13 @@
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -9732,13 +9744,13 @@
         <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -9749,13 +9761,13 @@
         <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -9766,13 +9778,13 @@
         <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E28" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -9783,13 +9795,13 @@
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D29" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="E29" s="33" t="s">
         <v>228</v>
-      </c>
-      <c r="E29" s="33" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -9800,13 +9812,13 @@
         <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E30" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -9817,13 +9829,13 @@
         <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -9834,13 +9846,13 @@
         <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -9851,13 +9863,13 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -9868,13 +9880,13 @@
         <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -9885,13 +9897,13 @@
         <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -9902,13 +9914,13 @@
         <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E36" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -10484,13 +10496,13 @@
       <selection activeCell="E45" sqref="B45:E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="51.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="51.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="25" customFormat="1" ht="18">
@@ -10758,10 +10770,10 @@
         <v>68</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -10772,10 +10784,10 @@
         <v>68</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -10786,10 +10798,10 @@
         <v>68</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -10800,10 +10812,10 @@
         <v>68</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -10814,10 +10826,10 @@
         <v>68</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -10828,10 +10840,10 @@
         <v>68</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -10842,10 +10854,10 @@
         <v>68</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -10856,10 +10868,10 @@
         <v>68</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -10870,10 +10882,10 @@
         <v>68</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -10884,10 +10896,10 @@
         <v>68</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -10898,10 +10910,10 @@
         <v>68</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -10912,10 +10924,10 @@
         <v>68</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E28" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -10926,10 +10938,10 @@
         <v>68</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -10940,10 +10952,10 @@
         <v>68</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E30" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -10954,10 +10966,10 @@
         <v>68</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -10968,10 +10980,10 @@
         <v>68</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -10982,10 +10994,10 @@
         <v>68</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -10996,10 +11008,10 @@
         <v>68</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -11010,10 +11022,10 @@
         <v>68</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -11024,10 +11036,10 @@
         <v>68</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E36" s="33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -11038,10 +11050,10 @@
         <v>68</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E37" s="33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -11052,10 +11064,10 @@
         <v>68</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E38" s="33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -11066,10 +11078,10 @@
         <v>68</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E39" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -11080,10 +11092,10 @@
         <v>68</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E40" s="33" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -11094,10 +11106,10 @@
         <v>64</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E41" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -11108,10 +11120,10 @@
         <v>64</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E42" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -11122,10 +11134,10 @@
         <v>64</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -11136,10 +11148,10 @@
         <v>64</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E44" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -11645,17 +11657,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView topLeftCell="A45" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="51.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="51.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="25" customFormat="1" ht="18">
@@ -11924,10 +11936,10 @@
         <v>64</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -11938,10 +11950,10 @@
         <v>72</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -11952,10 +11964,10 @@
         <v>72</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -11966,10 +11978,10 @@
         <v>72</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -11980,10 +11992,10 @@
         <v>72</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -11994,10 +12006,10 @@
         <v>72</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -12008,10 +12020,10 @@
         <v>72</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -12022,10 +12034,10 @@
         <v>72</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -12036,10 +12048,10 @@
         <v>72</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -12050,10 +12062,10 @@
         <v>75</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -12064,10 +12076,10 @@
         <v>75</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -12078,10 +12090,10 @@
         <v>75</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E28" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -12092,10 +12104,10 @@
         <v>75</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -12106,10 +12118,10 @@
         <v>75</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E30" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -12120,10 +12132,10 @@
         <v>75</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -12134,10 +12146,10 @@
         <v>75</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -12148,10 +12160,10 @@
         <v>75</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -12162,10 +12174,10 @@
         <v>75</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -12176,10 +12188,10 @@
         <v>75</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -12190,10 +12202,10 @@
         <v>75</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E36" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -12204,10 +12216,10 @@
         <v>75</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E37" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -12218,10 +12230,10 @@
         <v>75</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E38" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -12232,10 +12244,10 @@
         <v>75</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E39" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -12246,10 +12258,10 @@
         <v>75</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E40" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -12260,10 +12272,10 @@
         <v>75</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E41" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -12274,10 +12286,10 @@
         <v>75</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E42" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -12288,10 +12300,10 @@
         <v>75</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -12302,10 +12314,10 @@
         <v>75</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E44" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -12316,10 +12328,10 @@
         <v>75</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E45" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -12330,10 +12342,10 @@
         <v>75</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E46" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -12344,10 +12356,10 @@
         <v>75</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E47" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -12358,10 +12370,10 @@
         <v>72</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -12372,10 +12384,10 @@
         <v>84</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E49" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -12386,10 +12398,10 @@
         <v>79</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E50" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -12400,10 +12412,10 @@
         <v>79</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -12414,10 +12426,10 @@
         <v>79</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E52" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -12428,10 +12440,10 @@
         <v>79</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E53" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -12442,10 +12454,10 @@
         <v>79</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E54" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -12456,10 +12468,10 @@
         <v>79</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -12470,10 +12482,10 @@
         <v>88</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -12484,10 +12496,10 @@
         <v>88</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E57" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -12496,10 +12508,10 @@
       </c>
       <c r="B58" s="31"/>
       <c r="D58" s="31" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E58" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -12508,10 +12520,10 @@
       </c>
       <c r="B59" s="31"/>
       <c r="D59" s="31" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E59" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -12900,17 +12912,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="51.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="51.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="25" customFormat="1" ht="18">
@@ -12956,7 +12968,7 @@
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
@@ -13007,7 +13019,7 @@
       </c>
       <c r="B7" s="23">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
@@ -13022,7 +13034,7 @@
       </c>
       <c r="B8" s="23">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8" s="23">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -13040,7 +13052,7 @@
       </c>
       <c r="B9" s="23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C9" s="23">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -13058,7 +13070,7 @@
       </c>
       <c r="B10" s="23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10" s="23">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -13076,11 +13088,11 @@
       </c>
       <c r="B11" s="23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="23">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -13094,7 +13106,7 @@
       </c>
       <c r="B12" s="23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="23">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -13112,7 +13124,7 @@
       </c>
       <c r="B13" s="23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="23">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -13130,7 +13142,7 @@
       </c>
       <c r="B14" s="23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="23">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -13176,35 +13188,55 @@
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17" s="31"/>
+      <c r="B17" s="31" t="s">
+        <v>102</v>
+      </c>
       <c r="D17" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="E17" s="33"/>
+        <v>309</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="33"/>
+      <c r="B18" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
         <v>3</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="D19" s="31"/>
+      <c r="B19" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>311</v>
+      </c>
       <c r="E19" s="33"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
         <v>4</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="33"/>
+      <c r="B20" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
@@ -13910,19 +13942,19 @@
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="45.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="39.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="53.6640625" style="1" customWidth="1"/>
-    <col min="11" max="1024" width="11.5" style="1"/>
+    <col min="3" max="3" width="8.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="45.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="39.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="53.7109375" style="1" customWidth="1"/>
+    <col min="11" max="1024" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="18">
@@ -13942,7 +13974,7 @@
       </c>
       <c r="I1"/>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="16">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -14300,7 +14332,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
@@ -14326,7 +14358,7 @@
       </c>
       <c r="J24" s="15"/>
     </row>
-    <row r="25" spans="1:10" ht="14">
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -14352,7 +14384,7 @@
       </c>
       <c r="J25" s="15"/>
     </row>
-    <row r="26" spans="1:10" ht="14">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -14378,7 +14410,7 @@
       </c>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="1:10" ht="28">
+    <row r="27" spans="1:10" ht="38.25">
       <c r="A27" s="16" t="s">
         <v>41</v>
       </c>
@@ -14406,7 +14438,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="28">
+    <row r="28" spans="1:10" ht="25.5">
       <c r="A28" s="16" t="s">
         <v>45</v>
       </c>
@@ -14434,7 +14466,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="20" customFormat="1" ht="28">
+    <row r="29" spans="1:10" s="20" customFormat="1" ht="25.5">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -14462,7 +14494,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="20" customFormat="1" ht="28">
+    <row r="30" spans="1:10" s="20" customFormat="1" ht="25.5">
       <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
@@ -14490,7 +14522,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="20" customFormat="1" ht="28">
+    <row r="31" spans="1:10" s="20" customFormat="1" ht="25.5">
       <c r="A31" s="1" t="s">
         <v>55</v>
       </c>
@@ -14518,7 +14550,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="14">
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
         <v>57</v>
       </c>
@@ -14546,7 +14578,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:1024" ht="14">
+    <row r="33" spans="1:1024">
       <c r="A33" s="1" t="s">
         <v>62</v>
       </c>
@@ -14574,7 +14606,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:1024" ht="28">
+    <row r="34" spans="1:1024" ht="25.5">
       <c r="A34" s="16" t="s">
         <v>79</v>
       </c>
@@ -14596,13 +14628,13 @@
         <v>81</v>
       </c>
       <c r="I34" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="J34" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="J34" s="19" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1024" s="20" customFormat="1" ht="14">
+    </row>
+    <row r="35" spans="1:1024" s="20" customFormat="1">
       <c r="A35" s="16" t="s">
         <v>68</v>
       </c>
@@ -14628,7 +14660,7 @@
       </c>
       <c r="J35" s="19"/>
     </row>
-    <row r="36" spans="1:1024" s="20" customFormat="1" ht="14">
+    <row r="36" spans="1:1024" s="20" customFormat="1">
       <c r="A36" s="16" t="s">
         <v>75</v>
       </c>
@@ -14654,7 +14686,7 @@
       </c>
       <c r="J36" s="19"/>
     </row>
-    <row r="37" spans="1:1024" s="20" customFormat="1" ht="28">
+    <row r="37" spans="1:1024" s="20" customFormat="1" ht="38.25">
       <c r="A37" s="16" t="s">
         <v>84</v>
       </c>
@@ -14682,7 +14714,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:1024" s="20" customFormat="1" ht="28">
+    <row r="38" spans="1:1024" s="20" customFormat="1" ht="25.5">
       <c r="A38" s="16" t="s">
         <v>88</v>
       </c>
@@ -14710,7 +14742,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:1024" s="20" customFormat="1" ht="14">
+    <row r="39" spans="1:1024" s="20" customFormat="1" ht="25.5">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
@@ -14729,14 +14761,14 @@
         <v>69</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I39" s="15" t="s">
         <v>74</v>
       </c>
       <c r="J39" s="15"/>
     </row>
-    <row r="40" spans="1:1024" s="20" customFormat="1" ht="14">
+    <row r="40" spans="1:1024" s="20" customFormat="1">
       <c r="A40" s="1" t="s">
         <v>112</v>
       </c>
@@ -14762,7 +14794,7 @@
       </c>
       <c r="J40" s="15"/>
     </row>
-    <row r="41" spans="1:1024" s="22" customFormat="1" ht="28">
+    <row r="41" spans="1:1024" s="22" customFormat="1" ht="25.5">
       <c r="A41" s="1" t="s">
         <v>95</v>
       </c>
@@ -14790,7 +14822,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:1024" ht="28">
+    <row r="42" spans="1:1024" ht="25.5">
       <c r="A42" s="1" t="s">
         <v>99</v>
       </c>
@@ -15860,7 +15892,7 @@
       <c r="AMI43"/>
       <c r="AMJ43"/>
     </row>
-    <row r="44" spans="1:1024" ht="14">
+    <row r="44" spans="1:1024" ht="25.5">
       <c r="A44" s="16" t="s">
         <v>102</v>
       </c>
@@ -15925,7 +15957,7 @@
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
     </row>
-    <row r="48" spans="1:1024" ht="28">
+    <row r="48" spans="1:1024" ht="25.5">
       <c r="A48" s="1" t="s">
         <v>108</v>
       </c>
@@ -15951,7 +15983,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="14">
+    <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
         <v>115</v>
       </c>
@@ -15975,7 +16007,7 @@
       </c>
       <c r="J49" s="15"/>
     </row>
-    <row r="50" spans="1:10" ht="28">
+    <row r="50" spans="1:10" ht="38.25">
       <c r="A50" s="1" t="s">
         <v>118</v>
       </c>
@@ -15999,7 +16031,7 @@
       </c>
       <c r="J50" s="15"/>
     </row>
-    <row r="51" spans="1:10" ht="14">
+    <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
         <v>121</v>
       </c>
@@ -16023,7 +16055,7 @@
       </c>
       <c r="J51" s="15"/>
     </row>
-    <row r="52" spans="1:10" ht="28">
+    <row r="52" spans="1:10" ht="25.5">
       <c r="A52" s="1" t="s">
         <v>124</v>
       </c>
@@ -16047,7 +16079,7 @@
       </c>
       <c r="J52" s="15"/>
     </row>
-    <row r="53" spans="1:10" ht="14">
+    <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
         <v>127</v>
       </c>
@@ -16097,7 +16129,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="20" customFormat="1" ht="28">
+    <row r="55" spans="1:10" s="20" customFormat="1" ht="25.5">
       <c r="A55" s="1" t="s">
         <v>134</v>
       </c>
@@ -16123,7 +16155,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="28">
+    <row r="56" spans="1:10" ht="25.5">
       <c r="A56" s="1" t="s">
         <v>138</v>
       </c>
@@ -16147,7 +16179,7 @@
       </c>
       <c r="J56" s="15"/>
     </row>
-    <row r="57" spans="1:10" ht="28">
+    <row r="57" spans="1:10" ht="25.5">
       <c r="A57" s="1" t="s">
         <v>141</v>
       </c>
@@ -16171,7 +16203,7 @@
       </c>
       <c r="J57" s="15"/>
     </row>
-    <row r="58" spans="1:10" ht="28">
+    <row r="58" spans="1:10" ht="25.5">
       <c r="A58" s="1" t="s">
         <v>144</v>
       </c>
@@ -16195,7 +16227,7 @@
       </c>
       <c r="J58" s="15"/>
     </row>
-    <row r="59" spans="1:10" ht="28">
+    <row r="59" spans="1:10" ht="38.25">
       <c r="A59" s="1" t="s">
         <v>147</v>
       </c>
@@ -16219,7 +16251,7 @@
       </c>
       <c r="J59" s="15"/>
     </row>
-    <row r="60" spans="1:10" ht="14">
+    <row r="60" spans="1:10">
       <c r="A60" s="1" t="s">
         <v>150</v>
       </c>
@@ -16243,7 +16275,7 @@
       </c>
       <c r="J60" s="15"/>
     </row>
-    <row r="61" spans="1:10" ht="28">
+    <row r="61" spans="1:10" ht="25.5">
       <c r="A61" s="1" t="s">
         <v>152</v>
       </c>

</xml_diff>